<commit_message>
industry sector updates for BC and ON - changes from IESO project calibration
</commit_message>
<xml_diff>
--- a/csv/model/CIMS_FIC/formula_CIMS_FIC_AB.xlsx
+++ b/csv/model/CIMS_FIC/formula_CIMS_FIC_AB.xlsx
@@ -2,22 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\xCIMS\cims-models\csv\model\CIMS_FIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5C7D4E8-494D-45A9-ADC7-960BD92D713D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{98DFEABD-EFED-4428-A039-330A310FE51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1800" windowWidth="51840" windowHeight="21120" xr2:uid="{3B5DD806-B4BA-4D00-8E79-09DF27D35D15}"/>
+    <workbookView xWindow="34965" yWindow="3495" windowWidth="17250" windowHeight="8865" xr2:uid="{5D4BA253-E025-40A1-8B58-47B7BFDDB219}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -104,10 +101,10 @@
     <t>$</t>
   </si>
   <si>
-    <t>CIMS.CAN.AB.Natural Gas Extraction.Natural Gas.Exploration and Production.Conventional Production</t>
-  </si>
-  <si>
-    <t>Natural Gas Extraction</t>
+    <t>CIMS.CAN.AB.Natural Gas Production.Natural Gas.Exploration and Production.Conventional Production</t>
+  </si>
+  <si>
+    <t>Natural Gas Production</t>
   </si>
   <si>
     <t>Conventional Production</t>
@@ -122,7 +119,7 @@
     <t>Raw NG aggresive LDAR</t>
   </si>
   <si>
-    <t>CIMS.CAN.AB.Natural Gas Extraction.Natural Gas.Exploration and Production.Coal Bed Methane</t>
+    <t>CIMS.CAN.AB.Natural Gas Production.Natural Gas.Exploration and Production.Coal Bed Methane</t>
   </si>
   <si>
     <t>Coal Bed Methane</t>
@@ -131,7 +128,7 @@
     <t>Raw NG prod from coal bed methane Eff</t>
   </si>
   <si>
-    <t>CIMS.CAN.AB.Natural Gas Extraction.Natural Gas.Processing.Processing Plants</t>
+    <t>CIMS.CAN.AB.Natural Gas Production.Natural Gas.Processing.Processing Plants</t>
   </si>
   <si>
     <t>Processing Plants</t>
@@ -143,7 +140,7 @@
     <t>NG Eff</t>
   </si>
   <si>
-    <t>CIMS.CAN.AB.Natural Gas Extraction.Direct Heat</t>
+    <t>CIMS.CAN.AB.Natural Gas Production.Direct Heat</t>
   </si>
   <si>
     <t>Direct Heat</t>
@@ -155,7 +152,7 @@
     <t>Boilers improved thermal eff CCS</t>
   </si>
   <si>
-    <t>CIMS.CAN.AB.Natural Gas Extraction.Direct Drive Small</t>
+    <t>CIMS.CAN.AB.Natural Gas Production.Direct Drive Small</t>
   </si>
   <si>
     <t>Direct Drive Small</t>
@@ -1006,19 +1003,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="BC"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1337,7 +1321,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED49C271-D1FE-488D-A5DC-E7094F974861}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E500592F-FD7F-464B-8A50-F0CEC5943D7B}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:X166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2623,49 +2608,48 @@
       <c r="L20" t="s">
         <v>20</v>
       </c>
-      <c r="M20" t="e">
-        <f>[1]BC!$M$29</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N20" t="e">
+      <c r="M20">
+        <v>400000000</v>
+      </c>
+      <c r="N20">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="O20" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="O20">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="P20" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="P20">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="Q20" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="Q20">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="R20" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="R20">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="S20" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="S20">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="T20" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="T20">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="U20" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="U20">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="V20" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="V20">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="W20" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="W20">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
+        <v>400000000</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.3">
@@ -2693,49 +2677,48 @@
       <c r="L21" t="s">
         <v>20</v>
       </c>
-      <c r="M21" t="e">
-        <f>[1]BC!$M$30</f>
-        <v>#REF!</v>
-      </c>
-      <c r="N21" t="e">
+      <c r="M21">
+        <v>400000000</v>
+      </c>
+      <c r="N21">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="O21" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="O21">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="P21" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="P21">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="Q21" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="Q21">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="R21" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="R21">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="S21" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="S21">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="T21" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="T21">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="U21" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="U21">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="V21" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="V21">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
-      </c>
-      <c r="W21" t="e">
+        <v>400000000</v>
+      </c>
+      <c r="W21">
         <f t="shared" si="1"/>
-        <v>#REF!</v>
+        <v>400000000</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.3">
@@ -11928,7 +11911,7 @@
         <v>300</v>
       </c>
       <c r="N155">
-        <f t="shared" ref="N155:W158" si="10">M155</f>
+        <f t="shared" ref="N155:W156" si="10">M155</f>
         <v>300</v>
       </c>
       <c r="O155">

</xml_diff>

<commit_message>
updates from EMH project for policies (ZEV, clean elec, coal phase out, nuclear decom), transport personal (BEV 800 avail date), natural gas production (fix links)
</commit_message>
<xml_diff>
--- a/csv/model/CIMS_FIC/formula_CIMS_FIC_AB.xlsx
+++ b/csv/model/CIMS_FIC/formula_CIMS_FIC_AB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\xCIMS\cims-models\csv\model\CIMS_FIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{74CD84DA-8604-4991-AA16-698A01A74B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{147CAB0A-FF75-47CE-95F8-C5BB76D81A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A782CFEF-FFCD-4FC9-BFFF-3BF251137FF9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3B89ECF6-3FED-43AA-8B42-D89776D35B52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
     <t>$</t>
   </si>
   <si>
-    <t>CIMS.CAN.AB.Natural Gas Production.Natural Gas Supply.Processing.Processing Plants</t>
+    <t>CIMS.CAN.AB.Natural Gas Production.Supply.Processing.Processing Plants</t>
   </si>
   <si>
     <t>Natural Gas Production</t>
@@ -113,7 +113,7 @@
     <t>Processing</t>
   </si>
   <si>
-    <t>CIMS.CAN.AB.Natural Gas Production.Natural Gas Supply.Transmission</t>
+    <t>CIMS.CAN.AB.Natural Gas Production.Supply.Transmission</t>
   </si>
   <si>
     <t>Transmission</t>
@@ -122,7 +122,7 @@
     <t>Transmission HFO</t>
   </si>
   <si>
-    <t>CIMS.CAN.AB.Natural Gas Production.Natural Gas Supply.Direct Drive Small</t>
+    <t>CIMS.CAN.AB.Natural Gas Production.Supply.Direct Drive Small</t>
   </si>
   <si>
     <t>Direct Drive Small</t>
@@ -137,7 +137,7 @@
     <t>Reciprocating compressor electric</t>
   </si>
   <si>
-    <t>CIMS.CAN.AB.Natural Gas Production.Natural Gas Supply.Direct Drive Large</t>
+    <t>CIMS.CAN.AB.Natural Gas Production.Supply.Direct Drive Large</t>
   </si>
   <si>
     <t>Direct Drive Large</t>
@@ -152,7 +152,7 @@
     <t>Eff AC motor 500 hp</t>
   </si>
   <si>
-    <t>CIMS.CAN.AB.Natural Gas Production.Natural Gas Supply.Flaring</t>
+    <t>CIMS.CAN.AB.Natural Gas Production.Supply.Flaring</t>
   </si>
   <si>
     <t>Flaring</t>
@@ -161,7 +161,7 @@
     <t>No CCS</t>
   </si>
   <si>
-    <t>CIMS.CAN.AB.Natural Gas Production.Natural Gas Supply.Venting.Point Venting</t>
+    <t>CIMS.CAN.AB.Natural Gas Production.Supply.Venting.Point Venting</t>
   </si>
   <si>
     <t>Point Venting</t>
@@ -182,7 +182,7 @@
     <t>Ethanol</t>
   </si>
   <si>
-    <t>CIMS.CAN.AB.Natural Gas Production.Natural Gas Supply.Extraction.Off road transport</t>
+    <t>CIMS.CAN.AB.Natural Gas Production.Supply.Extraction.Off road transport</t>
   </si>
   <si>
     <t>Off road transport</t>
@@ -1531,7 +1531,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6A9AE4B-DAC1-42F6-B39E-58DEFCE3A9F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C813DCA-3305-422B-9617-9C1F38387C27}">
   <dimension ref="A1:X277"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">

</xml_diff>